<commit_message>
Replace commas with pipe symbol
</commit_message>
<xml_diff>
--- a/filepath_and_RIDs.xlsx
+++ b/filepath_and_RIDs.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B189"/>
+  <dimension ref="A1:B188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -373,7 +373,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RID49815, RID5720, RID3957, RID1560, RID35973, RID1559, RID8</t>
+          <t>RID49815 | RID5720 | RID3957 | RID1560 | RID35973 | RID1559 | RID8</t>
         </is>
       </c>
     </row>
@@ -385,7 +385,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RID49815, RID8, RID10409, RID49442, RID49572, RID11520, RID46056, RID34260, RID3957</t>
+          <t>RID49815 | RID8 | RID10409 | RID49442 | RID49572 | RID11520 | RID46056 | RID34260 | RID3957</t>
         </is>
       </c>
     </row>
@@ -397,7 +397,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>RID49815, RID8, RID36042, RID5821, RID3957, RID1560, RID1301, RID46056, RID38670, RID39348, RID4259, RID4247, RID5825, RID31011, RID7589, RID28474, RID6004, RID1430, RID28749, RID4226, RID6002, RID9970, RID5774, RID5824, RID6006, RID2507, RID237</t>
+          <t>RID49815 | RID8 | RID36042 | RID5821 | RID3957 | RID1560 | RID1301 | RID46056 | RID38670 | RID39348 | RID4259 | RID4247 | RID5825 | RID31011 | RID7589 | RID28474 | RID6004 | RID1430 | RID28749 | RID4226 | RID6002 | RID9970 | RID5774 | RID5824 | RID6006 | RID2507 | RID237</t>
         </is>
       </c>
     </row>
@@ -421,7 +421,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>RID39331, RID10337, RID13296, RID10341</t>
+          <t>RID39331 | RID10337 | RID13296 | RID10341</t>
         </is>
       </c>
     </row>
@@ -433,7 +433,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>RID49571, RID39252, RID10337, RID36026, RID38780, RID34301, RID45824, RID50374, RID50375, RID28816, RID45945, RID39262, RID5718</t>
+          <t>RID49571 | RID39252 | RID10337 | RID36026 | RID38780 | RID34301 | RID45824 | RID50374 | RID50375 | RID28816 | RID45945 | RID39262 | RID5718</t>
         </is>
       </c>
     </row>
@@ -457,7 +457,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>RID49815, RID5720, RID3957, RID1560, RID35973, RID1559, RID8</t>
+          <t>RID49815 | RID5720 | RID3957 | RID1560 | RID35973 | RID1559 | RID8</t>
         </is>
       </c>
     </row>
@@ -469,7 +469,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>RID49815, RID8, RID36042, RID5821, RID3957, RID1560, RID28474, RID7589, RID46056, RID290, RID15655, RID39348, RID5824</t>
+          <t>RID49815 | RID8 | RID36042 | RID5821 | RID3957 | RID1560 | RID28474 | RID7589 | RID46056 | RID290 | RID15655 | RID39348 | RID5824</t>
         </is>
       </c>
     </row>
@@ -481,7 +481,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>RID49815, RID8, RID10409, RID49442, RID49572, RID3957, RID5655, RID46056, RID11520, RID11513, RID5687, RID11515, RID39162, RID5689, RID45847</t>
+          <t>RID49815 | RID8 | RID10409 | RID49442 | RID49572 | RID3957 | RID5655 | RID46056 | RID11520 | RID11513 | RID5687 | RID11515 | RID39162 | RID5689 | RID45847</t>
         </is>
       </c>
     </row>
@@ -493,7 +493,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780, RID49834</t>
+          <t>RID5998 | RID5689 | RID45847 | RID3875 | RID38780 | RID49834</t>
         </is>
       </c>
     </row>
@@ -529,7 +529,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780, RID49834</t>
+          <t>RID5998 | RID5689 | RID45847 | RID3875 | RID38780 | RID49834</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
@@ -553,7 +553,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5998 | RID5689 | RID45847 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>RID5998, RID49834, RID3875, RID38780</t>
+          <t>RID5998 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834</t>
+          <t>RID5998 | RID5689 | RID45847 | RID49834</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780</t>
+          <t>RID5998 | RID5689 | RID45847 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
@@ -613,7 +613,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780</t>
+          <t>RID5998 | RID5689 | RID45847 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
@@ -625,7 +625,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5998 | RID5689 | RID45847 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
@@ -637,7 +637,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>RID5998, RID3875, RID38780, RID49834</t>
+          <t>RID5998 | RID3875 | RID38780 | RID49834</t>
         </is>
       </c>
     </row>
@@ -649,1975 +649,1963 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5998 | RID5689 | RID45847 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/055.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/125.xml</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5998 | RID5689 | RID45847 | RID49834</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/125.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/143.xml</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834</t>
+          <t>RID5998 | RID5689 | RID45847 | RID3875 | RID38780 | RID49834</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/143.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/157.xml</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780, RID49834</t>
+          <t>RID5998 | RID5689 | RID45847 | RID3875 | RID38780 | RID49834</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/157.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/142.xml</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780, RID49834</t>
+          <t>RID5998 | RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/142.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/175.xml</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847</t>
+          <t>RID5998 | RID5689 | RID45847 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/175.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/202.xml</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5998 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/202.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/204.xml</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>RID5998, RID49834, RID3875, RID38780</t>
+          <t>RID5998 | RID5689 | RID45847 | RID49834</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/204.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/060.xml</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834</t>
+          <t>RID5998 | RID5689 | RID45847 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/060.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/066.xml</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5998 | RID5689 | RID45847 | RID3875 | RID38780 | RID49834</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/066.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/138.xml</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780, RID49834</t>
+          <t>RID5998 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/138.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/110.xml</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>RID5998, RID49834, RID3875, RID38780</t>
+          <t>RID5998</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/110.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/044.xml</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>RID5998</t>
+          <t>RID5998 | RID5689 | RID45847 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/044.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/130.xml</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5998 | RID5689 | RID45847 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/130.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/157.xml</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780</t>
+          <t>RID5998 | RID5689 | RID45847 | RID3875 | RID38780 | RID49834</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/157.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/220.xml</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780, RID49834</t>
+          <t>RID5998 | RID5689 | RID45847 | RID3875 | RID38780 | RID49834</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/220.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/018.xml</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780, RID49834</t>
+          <t>RID5998 | RID5689 | RID45847 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/018.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/187.xml</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780</t>
+          <t>RID5998 | RID5689 | RID45847 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/187.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/033.xml</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5998 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/033.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/153.xml</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>RID5998, RID49834, RID3875, RID38780</t>
+          <t>RID5998 | RID3875 | RID38780 | RID49834</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/153.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/162.xml</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>RID5998, RID3875, RID38780, RID49834</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/162.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/176.xml</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/176.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/189.xml</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/189.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/201.xml</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/201.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/215.xml</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/215.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/163.xml</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/163.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/014.xml</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/014.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/202.xml</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/202.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/148.xml</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/148.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/158.xml</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/158.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/170.xml</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/170.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/164.xml</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5998 | RID5689 | RID45847 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/164.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/207.xml</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/207.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/159.xml</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/159.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/205.xml</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5998 | RID5689 | RID45847 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/205.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/204.xml</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/204.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/172.xml</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/172.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/166.xml</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/166.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/101.xml</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/101.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/115.xml</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/115.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/263.xml</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/263.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/060.xml</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/060.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/289.xml</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/289.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/100.xml</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/100.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/275.xml</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/275.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/271.xml</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/271.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/067.xml</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/067.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/066.xml</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/066.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/112.xml</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/112.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/104.xml</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/104.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/110.xml</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/110.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/299.xml</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/299.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/058.xml</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/058.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/267.xml</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/267.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/105.xml</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/105.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/139.xml</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/139.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/256.xml</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5998 | RID5689 | RID45847 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/256.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/082.xml</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/082.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/069.xml</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/069.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/280.xml</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/280.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/243.xml</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/243.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/241.xml</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/241.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/255.xml</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/255.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/296.xml</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/296.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/043.xml</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/043.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/240.xml</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/240.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/122.xml</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/122.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/136.xml</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/136.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/132.xml</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/132.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/278.xml</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/278.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/085.xml</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/085.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/292.xml</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/292.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/286.xml</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/286.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/245.xml</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/245.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/253.xml</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/253.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/290.xml</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/290.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/087.xml</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/087.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/044.xml</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5998 | RID5689 | RID45847 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/044.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/050.xml</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/050.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/285.xml</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/285.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/252.xml</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/252.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/180.xml</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/180.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/194.xml</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/194.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/209.xml</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/209.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/037.xml</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/037.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/234.xml</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/234.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/236.xml</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/236.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/008.xml</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/008.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/196.xml</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/196.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/145.xml</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/145.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/227.xml</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/227.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/150.xml</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/150.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/178.xml</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/178.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/033.xml</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/033.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/219.xml</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/219.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/190.xml</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/190.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/189.xml</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/189.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/214.xml</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/214.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/202.xml</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/202.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/158.xml</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/158.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/164.xml</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/164.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/213.xml</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/213.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/173.xml</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/173.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/239.xml</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/239.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/075.xml</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/075.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/289.xml</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/289.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/276.xml</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/276.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/128.xml</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/128.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/114.xml</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/114.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/116.xml</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/116.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/260.xml</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29, RID3875, RID38780</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/260.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/274.xml</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/274.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/249.xml</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/249.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/261.xml</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/261.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/271.xml</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/271.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/099.xml</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/099.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/264.xml</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/264.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/112.xml</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/112.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/104.xml</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/104.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/070.xml</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/070.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/267.xml</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/267.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/273.xml</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/273.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/120.xml</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/120.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/256.xml</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/256.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/068.xml</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/068.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/294.xml</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/294.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/109.xml</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/109.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/135.xml</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/135.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/241.xml</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/241.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/269.xml</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/269.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/095.xml</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/095.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/297.xml</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/297.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/268.xml</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5998 | RID5689 | RID45847 | RID49834 | RID3875 | RID38780</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/268.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/254.xml</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/254.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/122.xml</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/122.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/132.xml</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/132.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/084.xml</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/084.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/292.xml</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/292.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/247.xml</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/247.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/290.xml</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/290.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/284.xml</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/284.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/093.xml</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/093.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/124.xml</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/124.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/180.xml</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/180.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/235.xml</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/235.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/181.xml</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/181.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/183.xml</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/183.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/182.xml</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/182.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/196.xml</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/196.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/141.xml</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/141.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/179.xml</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/179.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/186.xml</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/186.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/227.xml</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/227.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/232.xml</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/232.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/185.xml</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/185.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/219.xml</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689 | RID45847 | RID29</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/219.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/184.xml</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689 | RID45847 | RID3875 | RID38780 | RID29</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/184.xml</t>
+          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_omf_v4.0_sarc.txt</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID49815 | RID8 | RID36042 | RID5821 | RID3957 | RID1560</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_omf_v4.0_sarc.txt</t>
+          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_follow_up_v4.0_nte_sarc.txt</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>RID49815, RID8, RID36042, RID5821, RID3957, RID1560</t>
+          <t>RID49815 | RID5720 | RID3957 | RID1560 | RID38780 | RID34301 | RID39123 | RID39144 | RID39066 | RID35973 | RID39068 | RID28492 | RID5727 | RID39330 | RID5972 | RID5703 | RID8 | RID1559 | RID58</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_follow_up_v4.0_nte_sarc.txt</t>
+          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_nte_sarc.txt</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>RID49815, RID5720, RID3957, RID1560, RID38780, RID34301, RID39123, RID39144, RID39066, RID35973, RID39068, RID28492, RID5727, RID39330, RID5972, RID5703, RID8, RID1559, RID58</t>
+          <t>RID49815 | RID5703 | RID28492 | RID3957 | RID5720 | RID1560 | RID38780 | RID34301 | RID39123 | RID39144 | RID39066 | RID35973 | RID5727 | RID39330 | RID5972 | RID39068 | RID8 | RID1559 | RID7741 | RID5833 | RID1301 | RID28474</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_nte_sarc.txt</t>
+          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_radiation_sarc.txt</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>RID49815, RID5703, RID28492, RID3957, RID5720, RID1560, RID38780, RID34301, RID39123, RID39144, RID39066, RID35973, RID5727, RID39330, RID5972, RID39068, RID8, RID1559, RID7741, RID5833, RID1301, RID28474</t>
+          <t>RID49815 | RID8 | RID10409 | RID49442 | RID49572 | RID3957 | RID11515 | RID39162 | RID46056</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_radiation_sarc.txt</t>
+          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_follow_up_v4.0_sarc.txt</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>RID49815, RID8, RID10409, RID49442, RID49572, RID3957, RID11515, RID39162, RID46056</t>
+          <t>RID49815 | RID8 | RID35973 | RID3957 | RID34658 | RID5720 | RID5729 | RID34616 | RID5655 | RID46056 | RID5689 | RID45847 | RID11514 | RID5734 | RID28474 | RID11515 | RID39162</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_follow_up_v4.0_sarc.txt</t>
+          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_drug_sarc.txt</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>RID49815, RID8, RID35973, RID3957, RID34658, RID5720, RID5729, RID34616, RID5655, RID46056, RID5689, RID45847, RID11514, RID5734, RID28474, RID11515, RID39162</t>
+          <t>RID49815 | RID35973 | RID8 | RID28492 | RID10409 | RID49442</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_drug_sarc.txt</t>
+          <t>NSCLC-Radiomics-Interobserver1/NSCLC-Radiomics-Interobserver1_ClinicalData.csv</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>RID49815, RID35973, RID8, RID28492, RID10409, RID49442</t>
-        </is>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" t="inlineStr">
-        <is>
-          <t>NSCLC-Radiomics-Interobserver1/NSCLC-Radiomics-Interobserver1_ClinicalData.csv</t>
-        </is>
-      </c>
-      <c r="B189" t="inlineStr">
-        <is>
-          <t>RID5653, RID4226, RID5825, RID5974, RID5967, RID39348, RID4247, RID5824, RID5962, RID5654, RID5774, RID1301, RID34616, RID46057, RID5778, RID46058</t>
+          <t>RID5653 | RID4226 | RID5825 | RID5974 | RID5967 | RID39348 | RID4247 | RID5824 | RID5962 | RID5654 | RID5774 | RID1301 | RID34616 | RID46057 | RID5778 | RID46058</t>
         </is>
       </c>
     </row>

</xml_diff>